<commit_message>
Updating routes to handle variables
</commit_message>
<xml_diff>
--- a/api/static/ProjectManagement.xlsx
+++ b/api/static/ProjectManagement.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62498121-1AD0-4036-AD2E-7ADA80D02687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2624D3A3-CEAC-4838-A61A-A8A71F71F6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="22">
   <si>
     <t>Project</t>
   </si>
@@ -52,7 +52,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>PERT</t>
+    <t>PRF</t>
   </si>
   <si>
     <t>Abhinav</t>
@@ -88,7 +88,10 @@
     <t>Sprint-4</t>
   </si>
   <si>
-    <t xml:space="preserve">Project </t>
+    <t>CART</t>
+  </si>
+  <si>
+    <t>SVN</t>
   </si>
   <si>
     <t>StoryPoints</t>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1013,6 +1016,1064 @@
         <v>11</v>
       </c>
     </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="1">
+        <v>44929</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1020,10 +2081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB03AE98-FF6C-4098-BD45-C06A21BA9051}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,13 +2096,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1085,6 +2146,94 @@
         <v>18</v>
       </c>
       <c r="C5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding gantt chart route
</commit_message>
<xml_diff>
--- a/api/static/ProjectManagement.xlsx
+++ b/api/static/ProjectManagement.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2624D3A3-CEAC-4838-A61A-A8A71F71F6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66F59922-E46F-468A-BCBC-36D48928FAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="28">
   <si>
     <t>Project</t>
   </si>
@@ -67,9 +67,15 @@
     <t>Completed</t>
   </si>
   <si>
+    <t>Shishir</t>
+  </si>
+  <si>
     <t>S103 : Reduce JS error in SignUp Page</t>
   </si>
   <si>
+    <t>Siri</t>
+  </si>
+  <si>
     <t>S104 : Reduce JS error in ATC Page</t>
   </si>
   <si>
@@ -95,6 +101,18 @@
   </si>
   <si>
     <t>StoryPoints</t>
+  </si>
+  <si>
+    <t>CompleteDate</t>
+  </si>
+  <si>
+    <t>Sprint-5</t>
+  </si>
+  <si>
+    <t>Sprint-6</t>
+  </si>
+  <si>
+    <t>Sprint-7</t>
   </si>
 </sst>
 </file>
@@ -450,7 +468,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,7 +478,7 @@
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -515,10 +533,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -538,10 +556,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -564,7 +582,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -587,7 +605,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -607,16 +625,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1">
         <v>44929</v>
@@ -630,16 +648,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1">
         <v>44929</v>
@@ -653,16 +671,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1">
         <v>44929</v>
@@ -676,16 +694,16 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F10" s="1">
         <v>44929</v>
@@ -702,13 +720,13 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="1">
         <v>44929</v>
@@ -722,16 +740,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1">
         <v>44929</v>
@@ -745,16 +763,16 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1">
         <v>44929</v>
@@ -768,16 +786,16 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F14" s="1">
         <v>44929</v>
@@ -791,16 +809,16 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F15" s="1">
         <v>44929</v>
@@ -817,13 +835,13 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1">
         <v>44929</v>
@@ -837,16 +855,16 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1">
         <v>44929</v>
@@ -860,16 +878,16 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1">
         <v>44929</v>
@@ -886,13 +904,13 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1">
         <v>44929</v>
@@ -909,13 +927,13 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1">
         <v>44929</v>
@@ -929,16 +947,16 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F21" s="1">
         <v>44929</v>
@@ -952,16 +970,16 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F22" s="1">
         <v>44929</v>
@@ -975,16 +993,16 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F23" s="1">
         <v>44929</v>
@@ -998,16 +1016,16 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F24" s="1">
         <v>44929</v>
@@ -1018,7 +1036,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -1041,13 +1059,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -1064,13 +1082,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -1087,13 +1105,13 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -1110,13 +1128,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1133,19 +1151,19 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F30" s="1">
         <v>44929</v>
@@ -1156,19 +1174,19 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F31" s="1">
         <v>44929</v>
@@ -1179,19 +1197,19 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F32" s="1">
         <v>44929</v>
@@ -1202,19 +1220,19 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F33" s="1">
         <v>44929</v>
@@ -1225,19 +1243,19 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F34" s="1">
         <v>44929</v>
@@ -1248,19 +1266,19 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F35" s="1">
         <v>44929</v>
@@ -1271,19 +1289,19 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D36">
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F36" s="1">
         <v>44929</v>
@@ -1294,19 +1312,19 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F37" s="1">
         <v>44929</v>
@@ -1317,19 +1335,19 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F38" s="1">
         <v>44929</v>
@@ -1340,19 +1358,19 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D39">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1">
         <v>44929</v>
@@ -1363,19 +1381,19 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F40" s="1">
         <v>44929</v>
@@ -1386,19 +1404,19 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F41" s="1">
         <v>44929</v>
@@ -1409,19 +1427,19 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F42" s="1">
         <v>44929</v>
@@ -1432,19 +1450,19 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D43">
         <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F43" s="1">
         <v>44929</v>
@@ -1455,19 +1473,19 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D44">
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F44" s="1">
         <v>44929</v>
@@ -1478,19 +1496,19 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D45">
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F45" s="1">
         <v>44929</v>
@@ -1501,19 +1519,19 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D46">
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F46" s="1">
         <v>44929</v>
@@ -1524,19 +1542,19 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F47" s="1">
         <v>44929</v>
@@ -1547,10 +1565,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1570,13 +1588,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49">
         <v>5</v>
@@ -1593,13 +1611,13 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D50">
         <v>4</v>
@@ -1616,13 +1634,13 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1639,13 +1657,13 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D52">
         <v>5</v>
@@ -1662,19 +1680,19 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F53" s="1">
         <v>44929</v>
@@ -1685,19 +1703,19 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F54" s="1">
         <v>44929</v>
@@ -1708,19 +1726,19 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D55">
         <v>4</v>
       </c>
       <c r="E55" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F55" s="1">
         <v>44929</v>
@@ -1731,19 +1749,19 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D56">
         <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F56" s="1">
         <v>44929</v>
@@ -1754,19 +1772,19 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D57">
         <v>4</v>
       </c>
       <c r="E57" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F57" s="1">
         <v>44929</v>
@@ -1777,19 +1795,19 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D58">
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F58" s="1">
         <v>44929</v>
@@ -1800,19 +1818,19 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D59">
         <v>4</v>
       </c>
       <c r="E59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F59" s="1">
         <v>44929</v>
@@ -1823,19 +1841,19 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F60" s="1">
         <v>44929</v>
@@ -1846,19 +1864,19 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D61">
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F61" s="1">
         <v>44929</v>
@@ -1869,19 +1887,19 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D62">
         <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F62" s="1">
         <v>44929</v>
@@ -1892,19 +1910,19 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F63" s="1">
         <v>44929</v>
@@ -1915,19 +1933,19 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D64">
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F64" s="1">
         <v>44929</v>
@@ -1938,19 +1956,19 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F65" s="1">
         <v>44929</v>
@@ -1961,19 +1979,19 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D66">
         <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F66" s="1">
         <v>44929</v>
@@ -1984,19 +2002,19 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D67">
         <v>5</v>
       </c>
       <c r="E67" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F67" s="1">
         <v>44929</v>
@@ -2007,19 +2025,19 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D68">
         <v>3</v>
       </c>
       <c r="E68" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F68" s="1">
         <v>44929</v>
@@ -2030,19 +2048,19 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D69">
         <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F69" s="1">
         <v>44929</v>
@@ -2053,19 +2071,19 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F70" s="1">
         <v>44929</v>
@@ -2081,20 +2099,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB03AE98-FF6C-4098-BD45-C06A21BA9051}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2102,10 +2120,16 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2115,126 +2139,317 @@
       <c r="C2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1">
+        <v>44935</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44946</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1">
+        <v>44949</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44960</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1">
+        <v>44963</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1">
+        <v>44977</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44991</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45005</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45047</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45061</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45075</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45086</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45089</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45103</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45117</v>
+      </c>
+      <c r="E13" s="1">
+        <v>45128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="C14">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44998</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45012</v>
+      </c>
+      <c r="E15" s="1">
+        <v>45023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
+      <c r="C16">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45026</v>
+      </c>
+      <c r="E16" s="1">
+        <v>45037</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
+      <c r="D17" s="1">
+        <v>45040</v>
+      </c>
+      <c r="E17" s="1">
+        <v>45051</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45054</v>
+      </c>
+      <c r="E18" s="1">
+        <v>45065</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45068</v>
+      </c>
+      <c r="E19" s="1">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>28</v>
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45082</v>
+      </c>
+      <c r="E20" s="1">
+        <v>45093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>